<commit_message>
Comentando os dados do relatório
</commit_message>
<xml_diff>
--- a/FlowShop_Genetic_Algorithm/reports/flow_shop_report.xlsx
+++ b/FlowShop_Genetic_Algorithm/reports/flow_shop_report.xlsx
@@ -14,36 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
-  <si>
-    <t>instances</t>
-  </si>
-  <si>
-    <t>solutions</t>
-  </si>
-  <si>
-    <t>lower_bound_f</t>
-  </si>
-  <si>
-    <t>upper_bound_f</t>
-  </si>
-  <si>
-    <t>mean_f</t>
-  </si>
-  <si>
-    <t>deviation_f</t>
-  </si>
-  <si>
-    <t>lower_bound_t</t>
-  </si>
-  <si>
-    <t>upper_bound_t</t>
-  </si>
-  <si>
-    <t>mean_t</t>
-  </si>
-  <si>
-    <t>deviation_t</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>Psize</t>
+  </si>
+  <si>
+    <t>sol</t>
+  </si>
+  <si>
+    <t>lbf</t>
+  </si>
+  <si>
+    <t>ubf</t>
+  </si>
+  <si>
+    <t>mf</t>
+  </si>
+  <si>
+    <t>dpf</t>
+  </si>
+  <si>
+    <t>lbt</t>
+  </si>
+  <si>
+    <t>ubt</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>dpt</t>
   </si>
   <si>
     <t>(20 X 5)</t>
@@ -76,34 +79,34 @@
     <t>(200 X 10)</t>
   </si>
   <si>
-    <t>[6, 5, 7, 3, 17, 8, 16, 15, 4, 19, 12, 2, 14, 11, 13, 9, 10, 1, 18, 20]</t>
-  </si>
-  <si>
-    <t>[5, 18, 12, 9, 4, 6, 14, 17, 19, 15, 13, 20, 11, 3, 7, 2, 8, 10, 1, 16]</t>
-  </si>
-  <si>
-    <t>[8, 16, 15, 18, 6, 20, 4, 11, 14, 17, 12, 13, 10, 9, 5, 7, 19, 2, 3, 1]</t>
-  </si>
-  <si>
-    <t>[31, 41, 50, 24, 48, 22, 29, 34, 1, 11, 6, 27, 10, 36, 39, 14, 15, 25, 4, 42, 38, 40, 21, 19, 20, 28, 2, 17, 23, 45, 18, 9, 13, 47, 49, 43, 26, 30, 3, 7, 8, 32, 12, 46, 44, 35, 5, 16, 33, 37]</t>
-  </si>
-  <si>
-    <t>[36, 48, 20, 6, 3, 33, 45, 8, 43, 49, 24, 30, 44, 14, 10, 22, 4, 28, 13, 34, 26, 16, 29, 11, 42, 46, 31, 19, 37, 32, 40, 39, 17, 5, 18, 35, 2, 41, 25, 7, 38, 9, 47, 1, 27, 21, 15, 50, 12, 23]</t>
-  </si>
-  <si>
-    <t>[35, 17, 20, 12, 25, 50, 1, 38, 5, 2, 9, 31, 43, 34, 45, 10, 6, 14, 41, 29, 28, 15, 7, 39, 46, 40, 16, 23, 8, 27, 22, 30, 49, 4, 24, 36, 42, 26, 33, 3, 44, 47, 48, 11, 19, 21, 13, 18, 37, 32]</t>
-  </si>
-  <si>
-    <t>[52, 85, 45, 70, 48, 84, 42, 28, 10, 16, 72, 18, 81, 2, 33, 65, 26, 57, 50, 64, 49, 38, 86, 9, 24, 55, 34, 77, 93, 6, 89, 31, 60, 100, 83, 96, 58, 66, 25, 47, 40, 54, 13, 78, 7, 61, 14, 44, 37, 82, 75, 68, 30, 90, 39, 4, 43, 8, 97, 41, 53, 36, 11, 5, 51, 56, 62, 69, 59, 1, 94, 12, 27, 15, 80, 95, 74, 63, 3, 19, 29, 99, 17, 32, 87, 67, 91, 73, 35, 46, 79, 22, 20, 21, 98, 71, 88, 23, 92, 76]</t>
-  </si>
-  <si>
-    <t>[15, 60, 37, 83, 50, 77, 12, 73, 4, 20, 24, 40, 42, 85, 17, 67, 13, 84, 21, 96, 65, 6, 16, 2, 8, 53, 74, 76, 81, 46, 39, 93, 51, 10, 89, 9, 38, 34, 88, 43, 5, 35, 47, 80, 14, 90, 99, 30, 94, 72, 95, 87, 100, 55, 22, 27, 91, 61, 75, 66, 82, 3, 92, 49, 28, 7, 62, 70, 98, 79, 69, 58, 97, 32, 71, 23, 86, 45, 36, 1, 19, 44, 78, 59, 48, 57, 68, 64, 29, 56, 33, 63, 31, 26, 41, 11, 54, 25, 18, 52]</t>
-  </si>
-  <si>
-    <t>[41, 78, 25, 59, 65, 58, 55, 4, 5, 27, 63, 86, 93, 33, 22, 10, 14, 31, 79, 32, 46, 70, 39, 54, 95, 16, 87, 49, 45, 3, 36, 68, 97, 1, 8, 20, 26, 82, 24, 2, 66, 85, 80, 74, 76, 43, 81, 7, 6, 40, 23, 52, 98, 57, 44, 61, 73, 21, 9, 64, 62, 94, 91, 17, 38, 71, 28, 19, 90, 56, 48, 88, 12, 89, 96, 83, 13, 34, 11, 53, 35, 84, 75, 51, 42, 60, 18, 100, 37, 50, 99, 69, 67, 72, 15, 30, 29, 47, 77, 92]</t>
-  </si>
-  <si>
-    <t>[34, 41, 190, 109, 11, 36, 33, 57, 6, 188, 100, 154, 38, 80, 137, 198, 110, 175, 114, 136, 187, 151, 96, 142, 192, 99, 44, 31, 85, 176, 155, 77, 82, 162, 152, 135, 174, 165, 4, 1, 131, 128, 143, 95, 12, 164, 180, 3, 148, 113, 120, 42, 117, 58, 20, 53, 184, 153, 66, 183, 146, 189, 166, 79, 92, 112, 94, 122, 196, 159, 185, 35, 163, 132, 181, 119, 48, 182, 45, 169, 173, 103, 59, 93, 102, 108, 55, 172, 160, 101, 105, 60, 88, 19, 5, 178, 43, 106, 28, 29, 2, 158, 84, 25, 46, 39, 72, 78, 121, 69, 87, 123, 116, 129, 56, 37, 81, 133, 70, 76, 18, 140, 167, 13, 86, 124, 126, 149, 32, 73, 89, 98, 26, 195, 156, 144, 7, 197, 171, 138, 161, 61, 65, 193, 40, 62, 107, 179, 90, 130, 125, 134, 22, 118, 150, 50, 16, 74, 17, 30, 191, 200, 168, 52, 127, 186, 8, 147, 14, 23, 71, 64, 91, 194, 75, 54, 21, 68, 9, 67, 63, 170, 139, 27, 24, 115, 157, 15, 83, 104, 141, 47, 145, 111, 177, 49, 51, 97, 10, 199]</t>
+    <t>[3, 15, 8, 4, 1, 17, 5, 19, 11, 13, 6, 14, 9, 12, 7, 18, 2, 20, 16, 10]</t>
+  </si>
+  <si>
+    <t>[9, 18, 6, 19, 17, 20, 14, 5, 10, 13, 4, 7, 8, 12, 15, 3, 2, 11, 16, 1]</t>
+  </si>
+  <si>
+    <t>[8, 18, 13, 15, 11, 6, 12, 7, 14, 10, 5, 19, 16, 9, 1, 2, 20, 4, 3, 17]</t>
+  </si>
+  <si>
+    <t>[3, 32, 39, 48, 4, 45, 22, 24, 26, 43, 10, 44, 16, 34, 42, 7, 35, 41, 20, 11, 28, 6, 1, 31, 19, 14, 5, 8, 9, 29, 13, 38, 12, 30, 2, 40, 18, 33, 46, 25, 47, 50, 37, 15, 23, 17, 27, 49, 21, 36]</t>
+  </si>
+  <si>
+    <t>[22, 32, 29, 20, 14, 40, 28, 49, 39, 34, 8, 44, 46, 15, 42, 48, 9, 36, 38, 3, 2, 5, 12, 24, 17, 19, 43, 13, 6, 47, 26, 25, 35, 16, 41, 4, 37, 50, 33, 10, 31, 21, 23, 27, 7, 18, 11, 1, 30, 45]</t>
+  </si>
+  <si>
+    <t>[12, 39, 6, 33, 41, 20, 31, 29, 28, 35, 21, 5, 47, 8, 26, 25, 43, 45, 48, 14, 17, 37, 40, 32, 16, 2, 10, 7, 38, 24, 49, 1, 15, 27, 44, 46, 11, 4, 36, 13, 9, 22, 30, 19, 42, 50, 23, 34, 18, 3]</t>
+  </si>
+  <si>
+    <t>[59, 16, 96, 73, 11, 40, 49, 74, 4, 26, 95, 99, 29, 19, 18, 1, 6, 25, 48, 41, 8, 42, 27, 90, 70, 13, 65, 93, 45, 88, 57, 24, 30, 68, 22, 10, 78, 38, 63, 92, 64, 75, 100, 2, 17, 97, 77, 61, 43, 60, 98, 72, 81, 62, 69, 12, 51, 55, 83, 33, 46, 44, 67, 54, 34, 94, 14, 35, 47, 56, 31, 89, 32, 39, 20, 5, 7, 36, 23, 71, 50, 76, 58, 3, 9, 86, 79, 87, 52, 53, 15, 21, 28, 85, 84, 37, 82, 91, 80, 66]</t>
+  </si>
+  <si>
+    <t>[5, 91, 97, 67, 10, 41, 31, 35, 24, 68, 3, 48, 65, 12, 98, 63, 33, 29, 46, 90, 89, 74, 55, 36, 2, 40, 42, 26, 7, 78, 49, 70, 57, 58, 60, 8, 85, 50, 22, 53, 75, 87, 88, 30, 62, 9, 64, 92, 54, 86, 72, 47, 94, 18, 69, 66, 81, 84, 19, 13, 52, 44, 15, 80, 25, 99, 20, 73, 21, 39, 79, 1, 34, 45, 76, 82, 95, 4, 77, 28, 83, 23, 93, 96, 56, 51, 71, 11, 38, 43, 16, 100, 6, 17, 27, 32, 37, 14, 61, 59]</t>
+  </si>
+  <si>
+    <t>[22, 47, 46, 35, 62, 91, 41, 31, 48, 93, 3, 100, 83, 60, 16, 81, 1, 61, 96, 44, 23, 21, 89, 10, 79, 30, 14, 12, 65, 98, 5, 15, 52, 51, 4, 8, 78, 71, 28, 27, 33, 42, 67, 18, 11, 90, 95, 72, 56, 2, 88, 64, 24, 84, 87, 43, 74, 6, 97, 68, 40, 57, 55, 7, 99, 25, 36, 58, 73, 9, 53, 50, 86, 59, 13, 20, 77, 37, 19, 39, 80, 75, 94, 29, 17, 66, 38, 70, 34, 85, 54, 49, 69, 92, 82, 63, 45, 26, 32, 76]</t>
+  </si>
+  <si>
+    <t>[85, 44, 84, 124, 28, 172, 93, 71, 19, 135, 26, 143, 103, 70, 166, 115, 91, 130, 49, 181, 110, 162, 77, 148, 127, 194, 33, 123, 108, 89, 40, 75, 153, 174, 6, 63, 29, 66, 24, 97, 95, 111, 53, 167, 163, 13, 177, 74, 42, 23, 165, 151, 170, 178, 7, 64, 86, 83, 137, 147, 134, 92, 138, 132, 131, 67, 17, 34, 2, 184, 156, 119, 16, 139, 25, 57, 190, 20, 62, 54, 193, 60, 59, 14, 125, 52, 47, 22, 154, 8, 114, 113, 199, 45, 4, 43, 159, 105, 100, 142, 140, 56, 186, 81, 160, 198, 73, 157, 48, 12, 99, 117, 94, 80, 112, 200, 41, 197, 180, 118, 164, 87, 152, 68, 155, 182, 191, 120, 32, 79, 187, 188, 18, 107, 196, 27, 150, 176, 129, 168, 35, 30, 11, 88, 145, 101, 122, 61, 175, 158, 96, 98, 76, 39, 72, 189, 51, 149, 109, 126, 161, 173, 136, 128, 171, 65, 116, 9, 3, 195, 106, 37, 10, 144, 102, 58, 5, 141, 31, 146, 55, 192, 90, 69, 36, 82, 21, 169, 38, 104, 179, 46, 121, 15, 185, 183, 50, 78, 1, 133]</t>
   </si>
 </sst>
 </file>
@@ -461,13 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -498,355 +501,388 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2">
-        <v>1324</v>
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>1377</v>
+        <v>1339</v>
       </c>
       <c r="F2">
-        <v>1352.9</v>
+        <v>1370</v>
       </c>
       <c r="G2">
-        <v>17.45537</v>
+        <v>1356.4</v>
       </c>
       <c r="H2">
-        <v>0.02631</v>
+        <v>10.46136</v>
       </c>
       <c r="I2">
-        <v>0.06232</v>
+        <v>0.02586</v>
       </c>
       <c r="J2">
-        <v>0.03663</v>
+        <v>0.05069</v>
       </c>
       <c r="K2">
-        <v>0.01007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>0.03714</v>
+      </c>
+      <c r="L2">
+        <v>0.00776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>1748</v>
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
       <c r="E3">
-        <v>1823</v>
+        <v>1756</v>
       </c>
       <c r="F3">
-        <v>1794.2</v>
+        <v>1824</v>
       </c>
       <c r="G3">
-        <v>23.60424</v>
+        <v>1793</v>
       </c>
       <c r="H3">
-        <v>0.04159</v>
+        <v>20.05492</v>
       </c>
       <c r="I3">
-        <v>0.10156</v>
+        <v>0.04141</v>
       </c>
       <c r="J3">
-        <v>0.07209</v>
+        <v>0.08833000000000001</v>
       </c>
       <c r="K3">
-        <v>0.01706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>0.06091</v>
+      </c>
+      <c r="L3">
+        <v>0.01544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
         <v>2499</v>
       </c>
-      <c r="E4">
-        <v>2556</v>
-      </c>
       <c r="F4">
-        <v>2522</v>
+        <v>2543</v>
       </c>
       <c r="G4">
-        <v>17.96664</v>
+        <v>2518.7</v>
       </c>
       <c r="H4">
-        <v>0.0737</v>
+        <v>13.22157</v>
       </c>
       <c r="I4">
-        <v>0.17031</v>
+        <v>0.07317</v>
       </c>
       <c r="J4">
-        <v>0.11307</v>
+        <v>0.15647</v>
       </c>
       <c r="K4">
-        <v>0.03086</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>0.09739</v>
+      </c>
+      <c r="L4">
+        <v>0.02938</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5">
-        <v>2810</v>
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
       </c>
       <c r="E5">
-        <v>2915</v>
+        <v>2845</v>
       </c>
       <c r="F5">
-        <v>2862.3</v>
+        <v>2909</v>
       </c>
       <c r="G5">
-        <v>25.96941</v>
+        <v>2870.3</v>
       </c>
       <c r="H5">
-        <v>0.05722</v>
+        <v>20.61577</v>
       </c>
       <c r="I5">
-        <v>0.15553</v>
+        <v>0.05755</v>
       </c>
       <c r="J5">
-        <v>0.09674000000000001</v>
+        <v>0.19922</v>
       </c>
       <c r="K5">
-        <v>0.03753</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>0.09457</v>
+      </c>
+      <c r="L5">
+        <v>0.04088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>3456</v>
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>3558</v>
+        <v>3467</v>
       </c>
       <c r="F6">
-        <v>3517.1</v>
+        <v>3555</v>
       </c>
       <c r="G6">
-        <v>30.8365</v>
+        <v>3509.5</v>
       </c>
       <c r="H6">
-        <v>0.09301</v>
+        <v>27.15971</v>
       </c>
       <c r="I6">
-        <v>0.28</v>
+        <v>0.09274</v>
       </c>
       <c r="J6">
-        <v>0.15693</v>
+        <v>0.21647</v>
       </c>
       <c r="K6">
-        <v>0.06226</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>0.13608</v>
+      </c>
+      <c r="L6">
+        <v>0.0386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7">
-        <v>4463</v>
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
       <c r="E7">
-        <v>4590</v>
+        <v>4454</v>
       </c>
       <c r="F7">
-        <v>4557</v>
+        <v>4594</v>
       </c>
       <c r="G7">
-        <v>35.08276</v>
+        <v>4548.9</v>
       </c>
       <c r="H7">
-        <v>0.1691</v>
+        <v>39.91854</v>
       </c>
       <c r="I7">
-        <v>0.38866</v>
+        <v>0.16541</v>
       </c>
       <c r="J7">
-        <v>0.2581</v>
+        <v>0.5809800000000001</v>
       </c>
       <c r="K7">
-        <v>0.06193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>0.26541</v>
+      </c>
+      <c r="L7">
+        <v>0.11976</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>5686</v>
+        <v>17</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
       </c>
       <c r="E8">
-        <v>5785</v>
+        <v>5659</v>
       </c>
       <c r="F8">
-        <v>5730.6</v>
+        <v>5805</v>
       </c>
       <c r="G8">
-        <v>27.98285</v>
+        <v>5735.2</v>
       </c>
       <c r="H8">
-        <v>0.10777</v>
+        <v>41.33957</v>
       </c>
       <c r="I8">
-        <v>0.27284</v>
+        <v>0.10687</v>
       </c>
       <c r="J8">
-        <v>0.17015</v>
+        <v>0.22874</v>
       </c>
       <c r="K8">
-        <v>0.05301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>0.1684</v>
+      </c>
+      <c r="L8">
+        <v>0.04085</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>6333</v>
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
       </c>
       <c r="E9">
-        <v>6523</v>
+        <v>6450</v>
       </c>
       <c r="F9">
-        <v>6465.3</v>
+        <v>6539</v>
       </c>
       <c r="G9">
-        <v>54.90364</v>
+        <v>6489.1</v>
       </c>
       <c r="H9">
-        <v>0.1758</v>
+        <v>29.22482</v>
       </c>
       <c r="I9">
-        <v>0.46599</v>
+        <v>0.22186</v>
       </c>
       <c r="J9">
-        <v>0.30145</v>
+        <v>0.64014</v>
       </c>
       <c r="K9">
-        <v>0.09178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>0.3037</v>
+      </c>
+      <c r="L9">
+        <v>0.11625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>7383</v>
+        <v>19</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
       </c>
       <c r="E10">
-        <v>7431</v>
+        <v>7267</v>
       </c>
       <c r="F10">
-        <v>7401.3</v>
+        <v>7433</v>
       </c>
       <c r="G10">
-        <v>16.30368</v>
+        <v>7363.3</v>
       </c>
       <c r="H10">
-        <v>0.31954</v>
+        <v>51.90963</v>
       </c>
       <c r="I10">
-        <v>1.01344</v>
+        <v>0.31728</v>
       </c>
       <c r="J10">
-        <v>0.47075</v>
+        <v>0.91704</v>
       </c>
       <c r="K10">
-        <v>0.21312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+        <v>0.56482</v>
+      </c>
+      <c r="L10">
+        <v>0.18813</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11">
-        <v>11656</v>
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>11798</v>
+        <v>11695</v>
       </c>
       <c r="F11">
-        <v>11726.8</v>
+        <v>11818</v>
       </c>
       <c r="G11">
-        <v>48.54235</v>
+        <v>11757.5</v>
       </c>
       <c r="H11">
-        <v>0.35499</v>
+        <v>39.4924</v>
       </c>
       <c r="I11">
-        <v>1.02232</v>
+        <v>0.34006</v>
       </c>
       <c r="J11">
-        <v>0.53027</v>
+        <v>0.73146</v>
       </c>
       <c r="K11">
-        <v>0.20783</v>
+        <v>0.47815</v>
+      </c>
+      <c r="L11">
+        <v>0.11837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>